<commit_message>
Mise à jour mapping corps 6e252a7146deaedf3e4787c95fe2bf14b0736235
</commit_message>
<xml_diff>
--- a/mappingCorps/ig/StructureDefinition-fr-diagnostic-report-document.xlsx
+++ b/mappingCorps/ig/StructureDefinition-fr-diagnostic-report-document.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-02-03T11:02:09+00:00</t>
+    <t>2026-02-04T10:58:36+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -620,7 +620,7 @@
 </t>
   </si>
   <si>
-    <t>Type de résultat. Codee n LOINC.</t>
+    <t>Type de résultat</t>
   </si>
   <si>
     <t>A code or name that describes this diagnostic report.</t>

</xml_diff>